<commit_message>
fix fetch issues upload excel works
</commit_message>
<xml_diff>
--- a/assets/excelTest.xlsx
+++ b/assets/excelTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itzik\WebstormProjects\Hameorer-client\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D5BB50-575C-41F8-AFD7-94C064477CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8944CAD1-5B99-4B56-91EC-80423FA6D1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{5DF7FEAC-A371-4FC5-949C-06B48887A9EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>password</t>
   </si>
@@ -53,52 +53,16 @@
     <t>dani</t>
   </si>
   <si>
-    <t>yosi</t>
-  </si>
-  <si>
-    <t>riki</t>
-  </si>
-  <si>
-    <t>auk</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>dgsf</t>
-  </si>
-  <si>
-    <t>dgfsa</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
     <t>phonenumber</t>
   </si>
   <si>
-    <t>asd@gmail.com</t>
-  </si>
-  <si>
-    <t>asd1@gmail.com</t>
-  </si>
-  <si>
-    <t>asd2@gmail.com</t>
-  </si>
-  <si>
-    <t>asd3@gmail.com</t>
-  </si>
-  <si>
     <t>0543248342</t>
   </si>
   <si>
-    <t>0543248341</t>
-  </si>
-  <si>
-    <t>0543248340</t>
-  </si>
-  <si>
-    <t>0543248339</t>
+    <t>1asd@gmail.com23</t>
   </si>
 </sst>
 </file>
@@ -151,8 +115,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -468,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB224378-4682-44EB-B85B-445B48CECE2B}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,10 +457,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -509,72 +473,17 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>131313</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>141414</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>151515</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{863B418C-D9F3-45A8-97DD-C29F45C88487}"/>
-    <hyperlink ref="D3:D5" r:id="rId2" display="asd@gmail.com" xr:uid="{52F833AC-000D-457E-A232-59201B58BD62}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{F0F317C1-7280-44B9-A099-47A5A9ADDFE9}"/>
-    <hyperlink ref="D4" r:id="rId4" xr:uid="{2C05B671-063A-4357-8629-AA063F7647DE}"/>
-    <hyperlink ref="D5" r:id="rId5" xr:uid="{A20E8799-599D-49FD-82CE-43BCDA14C9B6}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{AA655F1A-278D-44BF-8677-FF7AF13EB692}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>